<commit_message>
actualizacion del reporte anexo 7 y se ha corregido el diseño del reporte suministro GNS LIV a Enel
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/mensual/BoletaMensualdeSuministrodeGNSdelLIVaEnel.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/mensual/BoletaMensualdeSuministrodeGNSdelLIVaEnel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27630"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollos\SP\APSS SP\ProyectoPrincipalAenza5\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\mensual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollos\SP\APSS SP\ProyectoPrincipalAenza6\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\mensual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACEB8F3-97AF-419E-9023-D7F28A85E82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06275426-AA86-44FC-A2A6-18F816F4D61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Componente_Items">Hoja1!$B$10:$E$11</definedName>
-    <definedName name="Composicion_Items">Hoja1!$B$5:$E$6</definedName>
+    <definedName name="Componente_Items">Hoja1!$B$13:$E$14</definedName>
+    <definedName name="Composicion_Items">Hoja1!$B$8:$E$9</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>{{item.Fecha}}</t>
   </si>
@@ -82,8 +82,34 @@
     <t>{{Comentarios}}</t>
   </si>
   <si>
-    <t>UNNA ENERGIA S.A.
-BOLETA DE SUMINISTRO DE GNS DEL LOTE IV A ENEL GENERACION PIURA S.A.</t>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UNNA ENERGIA S.A.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+BOLETA DE SUMINISTRO DE GNS DEL LOTE IV A ENEL GENERACION 
+PIURA S.A.</t>
+    </r>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -100,7 +126,7 @@
     <numFmt numFmtId="169" formatCode="General_)"/>
     <numFmt numFmtId="170" formatCode="0.0000_ ;[Red]\-0.0000\ "/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,14 +161,6 @@
       <scheme val="major"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Helvetica"/>
       <family val="2"/>
@@ -158,8 +176,31 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,18 +215,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <fgColor rgb="FFDAEEF3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -261,25 +296,85 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -389,17 +484,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="7" fillId="4" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="4" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -413,44 +502,60 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="7" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="6" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="8" fillId="4" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="6" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="7" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="9" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="10" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="11" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -461,6 +566,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="104">
@@ -571,6 +682,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFDAEEF3"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -586,16 +702,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1150620</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>60961</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>224790</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>97340</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1040130</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>82100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -624,7 +740,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2110740" y="3954781"/>
+          <a:off x="320040" y="5265421"/>
           <a:ext cx="1680210" cy="935539"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -637,15 +753,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>3389</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -673,8 +789,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="152400" y="91440"/>
-          <a:ext cx="811109" cy="320040"/>
+          <a:off x="91440" y="91440"/>
+          <a:ext cx="872069" cy="320040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -959,11 +1075,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:H13"/>
+  <dimension ref="B1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <pane ySplit="7" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -975,118 +1091,132 @@
     <col min="5" max="5" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="24" t="s">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C1" s="10"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+    </row>
+    <row r="3" spans="2:8" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-    </row>
-    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="15" t="s">
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+    </row>
+    <row r="4" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D5" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="16"/>
-    </row>
-    <row r="4" spans="2:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="4"/>
-      <c r="C4" s="11" t="s">
+      <c r="E5" s="31"/>
+    </row>
+    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+    </row>
+    <row r="7" spans="2:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="2"/>
+      <c r="C7" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E7" s="15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="8" t="s">
+    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="9"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="13" t="s">
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="16"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D10" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E10" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="1"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="22" t="s">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="1"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="14" t="s">
+      <c r="C13" s="25"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="3"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="21"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="19" t="s">
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="1"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="23" t="s">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="B10:D10"/>
+  <mergeCells count="5">
+    <mergeCell ref="C14:D14"/>
     <mergeCell ref="B13:D13"/>
-    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="D5:E5"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
ajustes de las observaciones del reporte GNS LIV a Enel
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/mensual/BoletaMensualdeSuministrodeGNSdelLIVaEnel.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/mensual/BoletaMensualdeSuministrodeGNSdelLIVaEnel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27816"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollos\SP\APSS SP\ProyectoPrincipalAenza6\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\mensual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollos\SP\APSS SP\ProyectoPrincipalAenza7\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\mensual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06275426-AA86-44FC-A2A6-18F816F4D61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74325C7-A4C1-4E73-9BCB-6219B7D678AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Componente_Items">Hoja1!$B$13:$E$14</definedName>
+    <definedName name="Componente_Items">Hoja1!$B$14:$E$15</definedName>
     <definedName name="Composicion_Items">Hoja1!$B$8:$E$9</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>{{item.Fecha}}</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Fecha</t>
   </si>
 </sst>
 </file>
@@ -220,7 +223,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -258,11 +261,43 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -272,49 +307,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -377,6 +369,30 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -486,20 +502,19 @@
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -508,7 +523,7 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="6" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -524,10 +539,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -546,18 +561,30 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="4" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="4" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="8" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="169" fontId="6" fillId="0" borderId="9" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="169" fontId="6" fillId="0" borderId="10" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="6" fillId="0" borderId="11" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -567,11 +594,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="104">
@@ -704,13 +731,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>60961</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1040130</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>82100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -805,6 +832,50 @@
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1973580</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>15164</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF00AF4C-5AEE-B55E-7543-AAA9DA3DB54E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="220980" y="6073140"/>
+          <a:ext cx="5318760" cy="609524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1075,11 +1146,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:H16"/>
+  <dimension ref="B1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1092,131 +1162,141 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C1" s="10"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="3" spans="2:8" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
     </row>
     <row r="4" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="C5" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="22"/>
     </row>
     <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
     </row>
     <row r="7" spans="2:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="2"/>
-      <c r="C7" s="12" t="s">
+      <c r="B7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="14" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="16"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="3"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="25"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="1"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="1"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="20" t="s">
+      <c r="C14" s="28"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="1"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="1"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="27" t="s">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B17:D17"/>
     <mergeCell ref="C3:E3"/>
-    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
nuevos cambios del reporte GNS LIV a Enel
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/mensual/BoletaMensualdeSuministrodeGNSdelLIVaEnel.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/mensual/BoletaMensualdeSuministrodeGNSdelLIVaEnel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollos\SP\APSS SP\ProyectoPrincipalAenza7\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\mensual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74325C7-A4C1-4E73-9BCB-6219B7D678AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870D4ABD-65C0-41A2-9F52-46366273B1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,11 +82,17 @@
     <t>{{Comentarios}}</t>
   </si>
   <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
         <u/>
-        <sz val="11"/>
+        <sz val="14"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -97,7 +103,7 @@
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
+        <sz val="14"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -107,12 +113,6 @@
 BOLETA DE SUMINISTRO DE GNS DEL LOTE IV A ENEL GENERACION 
 PIURA S.A.</t>
     </r>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Fecha</t>
   </si>
 </sst>
 </file>
@@ -129,7 +129,7 @@
     <numFmt numFmtId="169" formatCode="General_)"/>
     <numFmt numFmtId="170" formatCode="0.0000_ ;[Red]\-0.0000\ "/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +202,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -223,7 +240,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -273,59 +290,31 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -393,6 +382,88 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -502,7 +573,7 @@
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -514,16 +585,13 @@
     <xf numFmtId="170" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -539,11 +607,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -558,47 +623,56 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="4" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="4" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="4" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="4" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="13" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="4" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="6" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="7" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="169" fontId="6" fillId="0" borderId="8" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="6" fillId="0" borderId="9" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="6" fillId="0" borderId="10" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="104">
@@ -779,16 +853,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>91439</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3389</xdr:colOff>
+      <xdr:colOff>335604</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -816,8 +890,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="91440" y="91440"/>
-          <a:ext cx="872069" cy="320040"/>
+          <a:off x="91439" y="45720"/>
+          <a:ext cx="1204285" cy="441960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1149,7 +1223,7 @@
   <dimension ref="B1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1162,111 +1236,111 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C1" s="9"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-    </row>
-    <row r="3" spans="2:8" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-    </row>
-    <row r="4" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="21" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="3" spans="2:8" ht="55.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="34" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="34"/>
-      <c r="E5" s="22"/>
+      <c r="E5" s="19"/>
     </row>
     <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="7" spans="2:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="5" t="s">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="23" t="s">
         <v>8</v>
       </c>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="15"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="24"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
       <c r="E9" s="4"/>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="25"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="25"/>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="18"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="19" t="s">
+      <c r="C14" s="31"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="17" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="3"/>
@@ -1275,27 +1349,27 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="B3:E3"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B17:D17"/>
-    <mergeCell ref="C3:E3"/>
     <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>